<commit_message>
adicion códigos que cambiaron
adicion códigos que cambiaron
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/SolicitudGrafica_CN_06_08_CO_REC70.xlsx
+++ b/fuentes/contenidos/grado06/guion08/SolicitudGrafica_CN_06_08_CO_REC70.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\Sofía CN_06_08_CO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1080" windowWidth="35025" windowHeight="17235" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="1080" windowWidth="35020" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -559,59 +554,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>208909639</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> /  13711744  ---------  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">http://commons.wikimedia.org/wiki/Panthera_onca?uselang=es#/media/File:Panthera_onca_at_the_Toronto_Zoo_2.jpg  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">     --------   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://www.flickr.com/photos/mckaysavage/8809044797 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">214006684  /  </t>
     </r>
     <r>
@@ -673,6 +615,34 @@
   </si>
   <si>
     <t>Se requiere crear una imagen compuesta por estas cuatro fotografías</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>208909639</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> /  13711744  ---------  41203633       110496089 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
@@ -1916,13 +1886,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1935,7 +1905,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1943,20 +1913,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1969,15 +1925,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1990,7 +1946,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1998,20 +1954,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2026,13 +1968,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2045,7 +1987,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2053,20 +1995,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2081,13 +2009,13 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2100,7 +2028,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2108,20 +2036,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2134,13 +2048,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -2155,7 +2069,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2163,20 +2077,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2189,13 +2089,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1057275</xdr:colOff>
+          <xdr:colOff>1054100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>863600</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -2210,7 +2110,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2218,20 +2118,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2244,7 +2130,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -2265,7 +2151,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2273,20 +2159,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2619,31 +2491,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="45.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="26" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="34.83203125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="17" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.875" style="2"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2655,7 +2527,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
@@ -2672,7 +2544,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2689,7 +2561,7 @@
       <c r="I3" s="46"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="16.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2710,7 +2582,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16.5" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2732,7 +2604,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="16.5" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2745,7 +2617,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="30" t="s">
         <v>40</v>
@@ -2763,7 +2635,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="9" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2782,7 +2654,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="14.25" thickBot="1">
       <c r="A9" s="26" t="s">
         <v>2</v>
       </c>
@@ -2817,7 +2689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A10" s="70" t="s">
         <v>149</v>
       </c>
@@ -2852,12 +2724,12 @@
       <c r="J10" s="81"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="37.5" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>150</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="72" t="s">
         <v>158</v>
@@ -2889,7 +2761,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>151</v>
       </c>
@@ -2924,12 +2796,12 @@
       <c r="J12" s="75"/>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="34.5" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>152</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>158</v>
@@ -2961,12 +2833,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="12" customFormat="1" ht="77.25" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>153</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>158</v>
@@ -2995,15 +2867,15 @@
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="12" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="12" customFormat="1" ht="52.5" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>154</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="72" t="s">
         <v>158</v>
@@ -3035,7 +2907,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>155</v>
       </c>
@@ -3070,7 +2942,7 @@
       <c r="J16" s="77"/>
       <c r="K16" s="27"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="82"/>
       <c r="C17" s="72"/>
@@ -3083,7 +2955,7 @@
       <c r="J17" s="78"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="82"/>
       <c r="C18" s="72"/>
@@ -3096,7 +2968,7 @@
       <c r="J18" s="78"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="82"/>
       <c r="C19" s="72"/>
@@ -3109,7 +2981,7 @@
       <c r="J19" s="77"/>
       <c r="K19" s="80"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="73"/>
       <c r="C20" s="72"/>
@@ -3122,7 +2994,7 @@
       <c r="J20" s="75"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="70"/>
       <c r="B21" s="82"/>
       <c r="C21" s="72"/>
@@ -3135,7 +3007,7 @@
       <c r="J21" s="78"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="70"/>
       <c r="B22" s="73"/>
       <c r="C22" s="72"/>
@@ -3148,7 +3020,7 @@
       <c r="J22" s="79"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="70"/>
       <c r="B23" s="73"/>
       <c r="C23" s="72"/>
@@ -3161,7 +3033,7 @@
       <c r="J23" s="75"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="70"/>
       <c r="B24" s="82"/>
       <c r="C24" s="72"/>
@@ -3174,7 +3046,7 @@
       <c r="J24" s="72"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="70"/>
       <c r="B25" s="74"/>
       <c r="C25" s="72"/>
@@ -3187,7 +3059,7 @@
       <c r="J25" s="72"/>
       <c r="K25" s="75"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="70"/>
       <c r="B26" s="74"/>
       <c r="C26" s="72"/>
@@ -3200,7 +3072,7 @@
       <c r="J26" s="72"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="70"/>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
@@ -3213,7 +3085,7 @@
       <c r="J27" s="75"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="70"/>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -3226,7 +3098,7 @@
       <c r="J28" s="75"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="70"/>
       <c r="B29" s="25"/>
       <c r="C29" s="25"/>
@@ -3239,7 +3111,7 @@
       <c r="J29" s="75"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="70"/>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -3252,7 +3124,7 @@
       <c r="J30" s="75"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A31" s="70"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25"/>
@@ -3265,7 +3137,7 @@
       <c r="J31" s="75"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A32" s="70"/>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
@@ -3278,7 +3150,7 @@
       <c r="J32" s="75"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A33" s="70"/>
       <c r="B33" s="83"/>
       <c r="C33" s="25"/>
@@ -3291,7 +3163,7 @@
       <c r="J33" s="75"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A34" s="70"/>
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
@@ -3304,7 +3176,7 @@
       <c r="J34" s="75"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A35" s="70"/>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
@@ -3317,7 +3189,7 @@
       <c r="J35" s="72"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A36" s="70"/>
       <c r="B36" s="83"/>
       <c r="C36" s="25"/>
@@ -3330,7 +3202,7 @@
       <c r="J36" s="72"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A37" s="70"/>
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
@@ -3343,7 +3215,7 @@
       <c r="J37" s="84"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A38" s="70"/>
       <c r="B38" s="83"/>
       <c r="C38" s="25"/>
@@ -3356,7 +3228,7 @@
       <c r="J38" s="44"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A39" s="70"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
@@ -3369,7 +3241,7 @@
       <c r="J39" s="72"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A40" s="70"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -3382,7 +3254,7 @@
       <c r="J40" s="72"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A41" s="70"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -3395,7 +3267,7 @@
       <c r="J41" s="72"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A42" s="70"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -3408,7 +3280,7 @@
       <c r="J42" s="72"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A43" s="70"/>
       <c r="B43" s="25"/>
       <c r="C43" s="25"/>
@@ -3421,7 +3293,7 @@
       <c r="J43" s="72"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A44" s="70"/>
       <c r="B44" s="83"/>
       <c r="C44" s="25"/>
@@ -3434,7 +3306,7 @@
       <c r="J44" s="72"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A45" s="70"/>
       <c r="B45" s="25"/>
       <c r="C45" s="25"/>
@@ -3447,7 +3319,7 @@
       <c r="J45" s="72"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="12" customFormat="1" ht="45.75" customHeight="1">
       <c r="A46" s="70"/>
       <c r="B46" s="70"/>
       <c r="C46" s="25"/>
@@ -3460,7 +3332,7 @@
       <c r="J46" s="72"/>
       <c r="K46" s="75"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="12" customFormat="1" ht="44.25" customHeight="1">
       <c r="A47" s="70"/>
       <c r="B47" s="70"/>
       <c r="C47" s="25"/>
@@ -3473,7 +3345,7 @@
       <c r="J47" s="72"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A48" s="70"/>
       <c r="B48" s="13"/>
       <c r="C48" s="25"/>
@@ -3486,7 +3358,7 @@
       <c r="J48" s="72"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A49" s="70"/>
       <c r="B49" s="85"/>
       <c r="C49" s="25"/>
@@ -3499,7 +3371,7 @@
       <c r="J49" s="72"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="25"/>
@@ -3512,7 +3384,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="25"/>
@@ -3525,7 +3397,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="25"/>
@@ -3538,7 +3410,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="25"/>
@@ -3551,7 +3423,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="25"/>
@@ -3564,7 +3436,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="25"/>
@@ -3577,7 +3449,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="25"/>
@@ -3590,7 +3462,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="25"/>
@@ -3603,7 +3475,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="25"/>
@@ -3616,7 +3488,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="25"/>
@@ -3629,7 +3501,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="25"/>
@@ -3642,7 +3514,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="25"/>
@@ -3655,7 +3527,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="25"/>
@@ -3668,7 +3540,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="25"/>
@@ -3681,7 +3553,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="25"/>
@@ -3694,7 +3566,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="25"/>
@@ -3707,7 +3579,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="25"/>
@@ -3720,7 +3592,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="25"/>
@@ -3733,7 +3605,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="25"/>
@@ -3746,7 +3618,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="12" customFormat="1">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="25"/>
@@ -3759,7 +3631,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="12" customFormat="1">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="25"/>
@@ -3772,7 +3644,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="12" customFormat="1">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="25"/>
@@ -3785,7 +3657,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="12" customFormat="1">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="25"/>
@@ -3798,7 +3670,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="12" customFormat="1">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="25"/>
@@ -3811,7 +3683,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="12" customFormat="1">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="25"/>
@@ -3824,7 +3696,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="12" customFormat="1">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="25"/>
@@ -3837,7 +3709,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="12" customFormat="1">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="25"/>
@@ -3850,7 +3722,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="12" customFormat="1">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="25"/>
@@ -3863,7 +3735,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="12" customFormat="1">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="25"/>
@@ -3876,7 +3748,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="12" customFormat="1">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="25"/>
@@ -3889,7 +3761,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="12" customFormat="1">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="25"/>
@@ -3902,7 +3774,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="12" customFormat="1">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="25"/>
@@ -3915,7 +3787,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="12" customFormat="1">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="25"/>
@@ -3928,7 +3800,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="12" customFormat="1">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="25"/>
@@ -3941,7 +3813,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="12" customFormat="1">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="25"/>
@@ -3954,7 +3826,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="12" customFormat="1">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="25"/>
@@ -3967,7 +3839,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="12" customFormat="1">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="25"/>
@@ -3980,7 +3852,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="12" customFormat="1">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="25"/>
@@ -3993,7 +3865,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="12" customFormat="1">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="25"/>
@@ -4006,7 +3878,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="12" customFormat="1">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="25"/>
@@ -4019,7 +3891,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="12" customFormat="1">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="25"/>
@@ -4032,7 +3904,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="12" customFormat="1">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="25"/>
@@ -4045,7 +3917,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="12" customFormat="1">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="25"/>
@@ -4058,7 +3930,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="12" customFormat="1">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="25"/>
@@ -4071,7 +3943,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="12" customFormat="1">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="25"/>
@@ -4084,7 +3956,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="12" customFormat="1">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="25"/>
@@ -4097,7 +3969,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="12" customFormat="1">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="25"/>
@@ -4110,7 +3982,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="12" customFormat="1">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="25"/>
@@ -4123,7 +3995,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="12" customFormat="1">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="25"/>
@@ -4136,7 +4008,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="12" customFormat="1">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="25"/>
@@ -4149,7 +4021,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="12" customFormat="1">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="25"/>
@@ -4162,7 +4034,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="12" customFormat="1">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="25"/>
@@ -4175,7 +4047,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A102" s="13" t="str">
         <f t="shared" ref="A102:A108" si="2">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE(LEFT(A101,3),IF(MID(A101,4,2)+1&lt;10,CONCATENATE("0",MID(A101,4,2)+1),MID(A101,4,2)+1)),"")</f>
         <v/>
@@ -4206,7 +4078,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A103" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4237,7 +4109,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A104" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4268,7 +4140,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A105" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4299,7 +4171,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A106" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4330,7 +4202,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A107" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4361,7 +4233,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A108" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4443,7 +4315,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4454,25 +4326,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="72.125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="28"/>
-    <col min="3" max="3" width="13.875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="28" customWidth="1"/>
-    <col min="5" max="7" width="10.875" style="28"/>
+    <col min="1" max="1" width="72.1640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="28"/>
+    <col min="3" max="3" width="13.83203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="28" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="28"/>
     <col min="8" max="11" width="11" style="28" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="28"/>
+    <col min="12" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1">
       <c r="A1" s="104" t="s">
         <v>38</v>
       </c>
@@ -4482,7 +4354,7 @@
       <c r="E1" s="105"/>
       <c r="F1" s="106"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="36" t="s">
         <v>42</v>
       </c>
@@ -4494,7 +4366,7 @@
       <c r="E2" s="109"/>
       <c r="F2" s="38"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63">
       <c r="A3" s="39" t="s">
         <v>43</v>
       </c>
@@ -4518,7 +4390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="36" t="s">
         <v>44</v>
       </c>
@@ -4546,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1">
       <c r="A5" s="39" t="s">
         <v>45</v>
       </c>
@@ -4573,7 +4445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1">
       <c r="A6" s="36" t="s">
         <v>10</v>
       </c>
@@ -4595,7 +4467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="48" thickBot="1">
       <c r="A7" s="39" t="s">
         <v>11</v>
       </c>
@@ -4622,7 +4494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.25">
       <c r="A8" s="39" t="s">
         <v>53</v>
       </c>
@@ -4641,7 +4513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.25">
       <c r="A9" s="39" t="s">
         <v>12</v>
       </c>
@@ -4660,7 +4532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1">
       <c r="A10" s="40" t="s">
         <v>36</v>
       </c>
@@ -4679,7 +4551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="I11" s="28" t="s">
         <v>32</v>
       </c>
@@ -4690,7 +4562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1">
       <c r="I12" s="28" t="s">
         <v>37</v>
       </c>
@@ -4701,7 +4573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="104" t="s">
         <v>41</v>
       </c>
@@ -4720,7 +4592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1">
       <c r="A14" s="39"/>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
@@ -4737,7 +4609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="36" t="s">
         <v>46</v>
       </c>
@@ -4755,7 +4627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.25" customHeight="1">
       <c r="A16" s="39" t="s">
         <v>47</v>
       </c>
@@ -4779,7 +4651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32.25" customHeight="1" thickBot="1">
       <c r="A17" s="36" t="s">
         <v>44</v>
       </c>
@@ -4800,7 +4672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1">
       <c r="A18" s="39" t="s">
         <v>48</v>
       </c>
@@ -4821,7 +4693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="36" t="s">
         <v>10</v>
       </c>
@@ -4840,7 +4712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
       <c r="A20" s="40" t="s">
         <v>51</v>
       </c>
@@ -4862,7 +4734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="H21" s="28" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -4879,122 +4751,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="K22" s="28">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="K23" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="K24" s="28">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" s="28">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="K26" s="28">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="K27" s="28">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="K28" s="28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="K29" s="28">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="K30" s="28">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="K31" s="28">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="K32" s="28">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11">
       <c r="K33" s="28">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11">
       <c r="K34" s="28">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11">
       <c r="K35" s="28">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11">
       <c r="K36" s="28">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11">
       <c r="K37" s="28">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11">
       <c r="K38" s="28">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11">
       <c r="K39" s="28">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11">
       <c r="K40" s="28">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11">
       <c r="K41" s="28">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11">
       <c r="K42" s="28">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11">
       <c r="K43" s="28">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11">
       <c r="K44" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11">
       <c r="K45" s="28" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -5028,18 +4900,19 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5048,20 +4921,21 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5072,18 +4946,19 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5094,18 +4969,19 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5114,13 +4990,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -5128,6 +5004,7 @@
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5136,13 +5013,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1057275</xdr:colOff>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>863600</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -5150,6 +5027,7 @@
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -5158,7 +5036,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -5172,9 +5050,11 @@
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5193,23 +5073,23 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="28" customWidth="1"/>
-    <col min="2" max="2" width="22.125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="28"/>
-    <col min="5" max="5" width="11.625" style="28" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="28"/>
+    <col min="5" max="5" width="11.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="28" customWidth="1"/>
     <col min="7" max="7" width="11" style="28" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="28" customWidth="1"/>
-    <col min="9" max="9" width="22.125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="20.625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="28" customWidth="1"/>
     <col min="11" max="11" width="44.5" style="28" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="28"/>
+    <col min="12" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="118" t="s">
         <v>56</v>
       </c>
@@ -5237,7 +5117,7 @@
       <c r="I1" s="119"/>
       <c r="J1" s="119"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="118"/>
       <c r="B2" s="118"/>
       <c r="C2" s="118"/>
@@ -5255,7 +5135,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="49" customFormat="1">
       <c r="A3" s="48" t="s">
         <v>69</v>
       </c>
@@ -5279,7 +5159,7 @@
       <c r="I3" s="48"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="49" customFormat="1">
       <c r="A4" s="50" t="s">
         <v>57</v>
       </c>
@@ -5307,7 +5187,7 @@
       </c>
       <c r="J4" s="50"/>
     </row>
-    <row r="5" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="49" customFormat="1">
       <c r="A5" s="51" t="s">
         <v>77</v>
       </c>
@@ -5335,7 +5215,7 @@
       </c>
       <c r="J5" s="52"/>
     </row>
-    <row r="6" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="49" customFormat="1">
       <c r="A6" s="50" t="s">
         <v>58</v>
       </c>
@@ -5367,7 +5247,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="49" customFormat="1" ht="25.5">
       <c r="A7" s="50" t="s">
         <v>80</v>
       </c>
@@ -5395,7 +5275,7 @@
       </c>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="49" customFormat="1" ht="25.5">
       <c r="A8" s="50" t="s">
         <v>82</v>
       </c>
@@ -5423,7 +5303,7 @@
       </c>
       <c r="J8" s="50"/>
     </row>
-    <row r="9" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="49" customFormat="1">
       <c r="A9" s="50" t="s">
         <v>84</v>
       </c>
@@ -5451,7 +5331,7 @@
       </c>
       <c r="J9" s="50"/>
     </row>
-    <row r="10" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="49" customFormat="1">
       <c r="A10" s="50" t="s">
         <v>86</v>
       </c>
@@ -5477,7 +5357,7 @@
       </c>
       <c r="J10" s="50"/>
     </row>
-    <row r="11" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="49" customFormat="1" ht="25.5">
       <c r="A11" s="50" t="s">
         <v>89</v>
       </c>
@@ -5505,7 +5385,7 @@
       </c>
       <c r="J11" s="50"/>
     </row>
-    <row r="12" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="49" customFormat="1">
       <c r="A12" s="50" t="s">
         <v>91</v>
       </c>
@@ -5533,7 +5413,7 @@
       </c>
       <c r="J12" s="50"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="63">
       <c r="A13" s="53" t="s">
         <v>93</v>
       </c>
@@ -5560,7 +5440,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="53" t="s">
         <v>97</v>
       </c>
@@ -5584,7 +5464,7 @@
       </c>
       <c r="J14" s="53"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="31.5">
       <c r="A15" s="53" t="s">
         <v>99</v>
       </c>
@@ -5611,7 +5491,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="94.5">
       <c r="A16" s="55" t="s">
         <v>103</v>
       </c>
@@ -5640,7 +5520,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="25.5">
       <c r="A17" s="50" t="s">
         <v>106</v>
       </c>
@@ -5669,12 +5549,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="59" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="60" t="s">
         <v>113</v>
       </c>
@@ -5687,7 +5567,7 @@
       <c r="D21" s="61"/>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="63" t="s">
         <v>114</v>
       </c>
@@ -5700,7 +5580,7 @@
       <c r="D22" s="64"/>
       <c r="E22" s="64"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="63" t="s">
         <v>115</v>
       </c>
@@ -5713,7 +5593,7 @@
       <c r="D23" s="64"/>
       <c r="E23" s="64"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="31.5">
       <c r="A24" s="63" t="s">
         <v>116</v>
       </c>
@@ -5726,7 +5606,7 @@
       <c r="D24" s="64"/>
       <c r="E24" s="64"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="63" t="s">
         <v>117</v>
       </c>
@@ -5739,7 +5619,7 @@
       <c r="D25" s="64"/>
       <c r="E25" s="64"/>
     </row>
-    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="63">
       <c r="A26" s="63" t="s">
         <v>118</v>
       </c>

</xml_diff>